<commit_message>
Changes to upload the app
</commit_message>
<xml_diff>
--- a/Fondos.xlsx
+++ b/Fondos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="267">
   <si>
     <t>I</t>
   </si>
@@ -263,87 +263,81 @@
     <t>191219</t>
   </si>
   <si>
+    <t>191226</t>
+  </si>
+  <si>
+    <t>181011</t>
+  </si>
+  <si>
+    <t>180614</t>
+  </si>
+  <si>
+    <t>180419</t>
+  </si>
+  <si>
+    <t>171221</t>
+  </si>
+  <si>
+    <t>180104</t>
+  </si>
+  <si>
+    <t>190328</t>
+  </si>
+  <si>
+    <t>210520</t>
+  </si>
+  <si>
+    <t>190808</t>
+  </si>
+  <si>
+    <t>190627</t>
+  </si>
+  <si>
+    <t>190606</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CPO</t>
+  </si>
+  <si>
+    <t>UBD</t>
+  </si>
+  <si>
+    <t>ISHRS</t>
+  </si>
+  <si>
+    <t>12D</t>
+  </si>
+  <si>
+    <t>593072</t>
+  </si>
+  <si>
+    <t>3752101</t>
+  </si>
+  <si>
+    <t>3752102</t>
+  </si>
+  <si>
+    <t>3752103</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>211223</t>
+  </si>
+  <si>
+    <t>180328</t>
+  </si>
+  <si>
+    <t>220609</t>
+  </si>
+  <si>
     <t>191205</t>
   </si>
   <si>
-    <t>181011</t>
-  </si>
-  <si>
-    <t>180614</t>
-  </si>
-  <si>
-    <t>180419</t>
-  </si>
-  <si>
-    <t>171221</t>
-  </si>
-  <si>
-    <t>180104</t>
-  </si>
-  <si>
-    <t>190328</t>
-  </si>
-  <si>
-    <t>210520</t>
-  </si>
-  <si>
-    <t>191226</t>
-  </si>
-  <si>
-    <t>190808</t>
-  </si>
-  <si>
-    <t>190627</t>
-  </si>
-  <si>
-    <t>190606</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>CPO</t>
-  </si>
-  <si>
-    <t>UBD</t>
-  </si>
-  <si>
-    <t>ISHRS</t>
-  </si>
-  <si>
-    <t>181213</t>
-  </si>
-  <si>
-    <t>12D</t>
-  </si>
-  <si>
-    <t>593072</t>
-  </si>
-  <si>
-    <t>3752101</t>
-  </si>
-  <si>
-    <t>3752102</t>
-  </si>
-  <si>
-    <t>3752103</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>191003</t>
-  </si>
-  <si>
-    <t>211223</t>
-  </si>
-  <si>
-    <t>180328</t>
-  </si>
-  <si>
-    <t>220609</t>
-  </si>
-  <si>
     <t>251204</t>
   </si>
   <si>
@@ -374,10 +368,10 @@
     <t>100000</t>
   </si>
   <si>
-    <t>95520</t>
-  </si>
-  <si>
-    <t>1056191</t>
+    <t>95367</t>
+  </si>
+  <si>
+    <t>1056038</t>
   </si>
   <si>
     <t>1400000</t>
@@ -392,7 +386,7 @@
     <t>1000000</t>
   </si>
   <si>
-    <t>1600000</t>
+    <t>1500000</t>
   </si>
   <si>
     <t>4500000</t>
@@ -410,10 +404,10 @@
     <t>35088</t>
   </si>
   <si>
-    <t>8685925</t>
-  </si>
-  <si>
-    <t>32628106</t>
+    <t>7722454</t>
+  </si>
+  <si>
+    <t>31564635</t>
   </si>
   <si>
     <t>76933</t>
@@ -446,10 +440,10 @@
     <t>32344</t>
   </si>
   <si>
-    <t>1570</t>
-  </si>
-  <si>
-    <t>896231</t>
+    <t>415</t>
+  </si>
+  <si>
+    <t>895076</t>
   </si>
   <si>
     <t>296500</t>
@@ -461,10 +455,10 @@
     <t>1000</t>
   </si>
   <si>
-    <t>11961337.98</t>
-  </si>
-  <si>
-    <t>1001791.89</t>
+    <t>12031537.98</t>
+  </si>
+  <si>
+    <t>1002317.83</t>
   </si>
   <si>
     <t>1011066.81</t>
@@ -473,7 +467,7 @@
     <t>1002216.55</t>
   </si>
   <si>
-    <t>15312777.23</t>
+    <t>15383503.17</t>
   </si>
   <si>
     <t>17446</t>
@@ -524,10 +518,10 @@
     <t>13106</t>
   </si>
   <si>
-    <t>216868</t>
-  </si>
-  <si>
-    <t>416386</t>
+    <t>155268</t>
+  </si>
+  <si>
+    <t>354786</t>
   </si>
   <si>
     <t>2500000</t>
@@ -536,6 +530,9 @@
     <t>2462600</t>
   </si>
   <si>
+    <t>740000</t>
+  </si>
+  <si>
     <t>150000</t>
   </si>
   <si>
@@ -548,10 +545,10 @@
     <t>44826</t>
   </si>
   <si>
-    <t>1504852</t>
-  </si>
-  <si>
-    <t>9512278</t>
+    <t>1498962</t>
+  </si>
+  <si>
+    <t>9246388</t>
   </si>
   <si>
     <t>1390300</t>
@@ -560,7 +557,7 @@
     <t>3500000</t>
   </si>
   <si>
-    <t>501900</t>
+    <t>361900</t>
   </si>
   <si>
     <t>350000</t>
@@ -572,136 +569,136 @@
     <t>15425</t>
   </si>
   <si>
-    <t>537640</t>
-  </si>
-  <si>
-    <t>6545265</t>
-  </si>
-  <si>
-    <t>4750965</t>
-  </si>
-  <si>
-    <t>1921020</t>
-  </si>
-  <si>
-    <t>4006800</t>
-  </si>
-  <si>
-    <t>2509400</t>
-  </si>
-  <si>
-    <t>5014000</t>
-  </si>
-  <si>
-    <t>3005820</t>
-  </si>
-  <si>
-    <t>1258033.96</t>
-  </si>
-  <si>
-    <t>10109500</t>
-  </si>
-  <si>
-    <t>9561838.56</t>
-  </si>
-  <si>
-    <t>42137377.52</t>
-  </si>
-  <si>
-    <t>140422800</t>
-  </si>
-  <si>
-    <t>200972000</t>
-  </si>
-  <si>
-    <t>301497000</t>
-  </si>
-  <si>
-    <t>100097000</t>
-  </si>
-  <si>
-    <t>51441000</t>
-  </si>
-  <si>
-    <t>161752000</t>
-  </si>
-  <si>
-    <t>42758685</t>
-  </si>
-  <si>
-    <t>335757100</t>
-  </si>
-  <si>
-    <t>45490783.36</t>
-  </si>
-  <si>
-    <t>200508000</t>
-  </si>
-  <si>
-    <t>200606000</t>
-  </si>
-  <si>
-    <t>210217145.3</t>
-  </si>
-  <si>
-    <t>3505329.8</t>
-  </si>
-  <si>
-    <t>870798724.95</t>
-  </si>
-  <si>
-    <t>2865823568.41</t>
-  </si>
-  <si>
-    <t>4732918.16</t>
-  </si>
-  <si>
-    <t>5806721.48</t>
-  </si>
-  <si>
-    <t>5420279.2</t>
-  </si>
-  <si>
-    <t>7193873.24</t>
-  </si>
-  <si>
-    <t>5008014</t>
-  </si>
-  <si>
-    <t>3631162.5</t>
-  </si>
-  <si>
-    <t>4209610</t>
-  </si>
-  <si>
-    <t>5651007.6</t>
-  </si>
-  <si>
-    <t>5301754.48</t>
-  </si>
-  <si>
-    <t>5811246.48</t>
-  </si>
-  <si>
-    <t>157207.24</t>
-  </si>
-  <si>
-    <t>52923794.38</t>
-  </si>
-  <si>
-    <t>280774826</t>
-  </si>
-  <si>
-    <t>79679361.44</t>
-  </si>
-  <si>
-    <t>1856830</t>
-  </si>
-  <si>
-    <t>216911627.91</t>
-  </si>
-  <si>
-    <t>18995381.26</t>
+    <t>540626</t>
+  </si>
+  <si>
+    <t>6408251</t>
+  </si>
+  <si>
+    <t>4750830</t>
+  </si>
+  <si>
+    <t>1921136</t>
+  </si>
+  <si>
+    <t>4008800</t>
+  </si>
+  <si>
+    <t>2510425</t>
+  </si>
+  <si>
+    <t>5016150</t>
+  </si>
+  <si>
+    <t>3007110</t>
+  </si>
+  <si>
+    <t>1258547.2</t>
+  </si>
+  <si>
+    <t>10112800</t>
+  </si>
+  <si>
+    <t>9510598.05</t>
+  </si>
+  <si>
+    <t>42096396.25</t>
+  </si>
+  <si>
+    <t>140483000</t>
+  </si>
+  <si>
+    <t>199916400</t>
+  </si>
+  <si>
+    <t>299913600</t>
+  </si>
+  <si>
+    <t>100136000</t>
+  </si>
+  <si>
+    <t>51460000</t>
+  </si>
+  <si>
+    <t>151692000</t>
+  </si>
+  <si>
+    <t>42757470</t>
+  </si>
+  <si>
+    <t>335844200</t>
+  </si>
+  <si>
+    <t>45508776.83</t>
+  </si>
+  <si>
+    <t>199452600</t>
+  </si>
+  <si>
+    <t>199551000</t>
+  </si>
+  <si>
+    <t>210290699.97</t>
+  </si>
+  <si>
+    <t>3506722.79</t>
+  </si>
+  <si>
+    <t>770131764.34</t>
+  </si>
+  <si>
+    <t>2750644233.93</t>
+  </si>
+  <si>
+    <t>4738303.47</t>
+  </si>
+  <si>
+    <t>6047845.44</t>
+  </si>
+  <si>
+    <t>5294053.52</t>
+  </si>
+  <si>
+    <t>7313073.88</t>
+  </si>
+  <si>
+    <t>4997322</t>
+  </si>
+  <si>
+    <t>3619635</t>
+  </si>
+  <si>
+    <t>4259630</t>
+  </si>
+  <si>
+    <t>5763295.44</t>
+  </si>
+  <si>
+    <t>5338098.04</t>
+  </si>
+  <si>
+    <t>5999488.56</t>
+  </si>
+  <si>
+    <t>41386.41</t>
+  </si>
+  <si>
+    <t>53412131.76</t>
+  </si>
+  <si>
+    <t>281636158.5</t>
+  </si>
+  <si>
+    <t>79923816</t>
+  </si>
+  <si>
+    <t>1860470</t>
+  </si>
+  <si>
+    <t>218213873.01</t>
+  </si>
+  <si>
+    <t>18581469.09</t>
   </si>
   <si>
     <t>19513083.9</t>
@@ -710,112 +707,112 @@
     <t>18655559.53</t>
   </si>
   <si>
-    <t>636386670.04</t>
-  </si>
-  <si>
-    <t>56107557.22</t>
-  </si>
-  <si>
-    <t>51236031</t>
-  </si>
-  <si>
-    <t>9957610</t>
-  </si>
-  <si>
-    <t>9773351.07</t>
-  </si>
-  <si>
-    <t>7578305</t>
-  </si>
-  <si>
-    <t>10567005.02</t>
-  </si>
-  <si>
-    <t>12590857.59</t>
-  </si>
-  <si>
-    <t>42268389.2</t>
-  </si>
-  <si>
-    <t>10835649</t>
-  </si>
-  <si>
-    <t>26120655.36</t>
-  </si>
-  <si>
-    <t>19352454</t>
-  </si>
-  <si>
-    <t>28669728.6</t>
-  </si>
-  <si>
-    <t>43542237.9</t>
-  </si>
-  <si>
-    <t>10258156.15</t>
-  </si>
-  <si>
-    <t>26961454.66</t>
-  </si>
-  <si>
-    <t>45466942.02</t>
-  </si>
-  <si>
-    <t>21748824.25</t>
-  </si>
-  <si>
-    <t>433035208.04</t>
-  </si>
-  <si>
-    <t>24012750</t>
-  </si>
-  <si>
-    <t>23399452.82</t>
-  </si>
-  <si>
-    <t>101095000</t>
-  </si>
-  <si>
-    <t>15091050</t>
-  </si>
-  <si>
-    <t>60208200</t>
-  </si>
-  <si>
-    <t>125282500</t>
-  </si>
-  <si>
-    <t>25236455.26</t>
-  </si>
-  <si>
-    <t>150825296.55</t>
-  </si>
-  <si>
-    <t>525150704.63</t>
-  </si>
-  <si>
-    <t>13353970.53</t>
-  </si>
-  <si>
-    <t>33256755</t>
-  </si>
-  <si>
-    <t>50739580.5</t>
-  </si>
-  <si>
-    <t>35212450</t>
-  </si>
-  <si>
-    <t>25025750</t>
-  </si>
-  <si>
-    <t>10001415.75</t>
-  </si>
-  <si>
-    <t>53917765.04</t>
-  </si>
-  <si>
-    <t>221507686.82</t>
+    <t>638384430.03</t>
+  </si>
+  <si>
+    <t>55883027.2</t>
+  </si>
+  <si>
+    <t>50667540</t>
+  </si>
+  <si>
+    <t>10112960</t>
+  </si>
+  <si>
+    <t>9803335.5</t>
+  </si>
+  <si>
+    <t>7719005</t>
+  </si>
+  <si>
+    <t>10831021.76</t>
+  </si>
+  <si>
+    <t>12833986.01</t>
+  </si>
+  <si>
+    <t>39928888</t>
+  </si>
+  <si>
+    <t>11929920.75</t>
+  </si>
+  <si>
+    <t>27017637.6</t>
+  </si>
+  <si>
+    <t>20079121.5</t>
+  </si>
+  <si>
+    <t>28024178.7</t>
+  </si>
+  <si>
+    <t>42421254.75</t>
+  </si>
+  <si>
+    <t>10928384.72</t>
+  </si>
+  <si>
+    <t>27562761.98</t>
+  </si>
+  <si>
+    <t>43258712.08</t>
+  </si>
+  <si>
+    <t>15484303.15</t>
+  </si>
+  <si>
+    <t>424486038.7</t>
+  </si>
+  <si>
+    <t>24014200</t>
+  </si>
+  <si>
+    <t>23398787.92</t>
+  </si>
+  <si>
+    <t>74834720</t>
+  </si>
+  <si>
+    <t>15096600</t>
+  </si>
+  <si>
+    <t>60232200</t>
+  </si>
+  <si>
+    <t>125315000</t>
+  </si>
+  <si>
+    <t>25249947.89</t>
+  </si>
+  <si>
+    <t>149485934.1</t>
+  </si>
+  <si>
+    <t>497627389.91</t>
+  </si>
+  <si>
+    <t>13354776.9</t>
+  </si>
+  <si>
+    <t>33255810</t>
+  </si>
+  <si>
+    <t>36598223.2</t>
+  </si>
+  <si>
+    <t>35225400</t>
+  </si>
+  <si>
+    <t>25035750</t>
+  </si>
+  <si>
+    <t>10028872.25</t>
+  </si>
+  <si>
+    <t>53914630.66</t>
+  </si>
+  <si>
+    <t>207413463.01</t>
   </si>
 </sst>
 </file>
@@ -906,10 +903,10 @@
         <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
@@ -929,10 +926,10 @@
         <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4">
@@ -952,10 +949,10 @@
         <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5">
@@ -975,10 +972,10 @@
         <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6">
@@ -998,10 +995,10 @@
         <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7">
@@ -1021,10 +1018,10 @@
         <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8">
@@ -1044,7 +1041,7 @@
         <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
@@ -1067,10 +1064,10 @@
         <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
@@ -1090,10 +1087,10 @@
         <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11">
@@ -1113,10 +1110,10 @@
         <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12">
@@ -1136,10 +1133,10 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13">
@@ -1159,10 +1156,10 @@
         <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14">
@@ -1182,10 +1179,10 @@
         <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15">
@@ -1205,10 +1202,10 @@
         <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16">
@@ -1228,10 +1225,10 @@
         <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17">
@@ -1251,10 +1248,10 @@
         <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18">
@@ -1274,10 +1271,10 @@
         <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19">
@@ -1297,10 +1294,10 @@
         <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20">
@@ -1320,10 +1317,10 @@
         <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21">
@@ -1343,10 +1340,10 @@
         <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22">
@@ -1363,13 +1360,13 @@
         <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23">
@@ -1386,13 +1383,13 @@
         <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24">
@@ -1409,13 +1406,13 @@
         <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25">
@@ -1432,13 +1429,13 @@
         <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26">
@@ -1455,13 +1452,13 @@
         <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27">
@@ -1481,10 +1478,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28">
@@ -1504,10 +1501,10 @@
         <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29">
@@ -1524,13 +1521,13 @@
         <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30">
@@ -1547,13 +1544,13 @@
         <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31">
@@ -1573,10 +1570,10 @@
         <v>80</v>
       </c>
       <c r="F31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32">
@@ -1593,13 +1590,13 @@
         <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33">
@@ -1616,13 +1613,13 @@
         <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34">
@@ -1639,13 +1636,13 @@
         <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35">
@@ -1662,13 +1659,13 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36">
@@ -1688,10 +1685,10 @@
         <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37">
@@ -1708,13 +1705,13 @@
         <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38">
@@ -1731,13 +1728,13 @@
         <v>40</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39">
@@ -1757,10 +1754,10 @@
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40">
@@ -1780,10 +1777,10 @@
         <v>80</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41">
@@ -1803,10 +1800,10 @@
         <v>80</v>
       </c>
       <c r="F41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42">
@@ -1823,13 +1820,13 @@
         <v>55</v>
       </c>
       <c r="E42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43">
@@ -1846,13 +1843,13 @@
         <v>56</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44">
@@ -1869,13 +1866,13 @@
         <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45">
@@ -1892,13 +1889,13 @@
         <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46">
@@ -1915,13 +1912,13 @@
         <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47">
@@ -1941,10 +1938,10 @@
         <v>9</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48">
@@ -1964,10 +1961,10 @@
         <v>80</v>
       </c>
       <c r="F48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49">
@@ -1987,10 +1984,10 @@
         <v>80</v>
       </c>
       <c r="F49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50">
@@ -2010,10 +2007,10 @@
         <v>80</v>
       </c>
       <c r="F50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51">
@@ -2033,10 +2030,10 @@
         <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52">
@@ -2056,10 +2053,10 @@
         <v>80</v>
       </c>
       <c r="F52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53">
@@ -2079,10 +2076,10 @@
         <v>80</v>
       </c>
       <c r="F53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G53" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54">
@@ -2102,10 +2099,10 @@
         <v>80</v>
       </c>
       <c r="F54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G54" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55">
@@ -2125,10 +2122,10 @@
         <v>80</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56">
@@ -2148,10 +2145,10 @@
         <v>80</v>
       </c>
       <c r="F56" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57">
@@ -2171,10 +2168,10 @@
         <v>80</v>
       </c>
       <c r="F57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58">
@@ -2194,10 +2191,10 @@
         <v>80</v>
       </c>
       <c r="F58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G58" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59">
@@ -2217,10 +2214,10 @@
         <v>80</v>
       </c>
       <c r="F59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G59" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60">
@@ -2240,10 +2237,10 @@
         <v>80</v>
       </c>
       <c r="F60" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61">
@@ -2263,10 +2260,10 @@
         <v>80</v>
       </c>
       <c r="F61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62">
@@ -2286,10 +2283,10 @@
         <v>80</v>
       </c>
       <c r="F62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63">
@@ -2306,13 +2303,13 @@
         <v>72</v>
       </c>
       <c r="E63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F63" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="64">
@@ -2329,13 +2326,13 @@
         <v>40</v>
       </c>
       <c r="E64" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="F64" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65">
@@ -2355,10 +2352,10 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66">
@@ -2378,10 +2375,10 @@
         <v>75</v>
       </c>
       <c r="F66" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G66" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67">
@@ -2401,10 +2398,10 @@
         <v>74</v>
       </c>
       <c r="F67" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G67" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68">
@@ -2424,10 +2421,10 @@
         <v>82</v>
       </c>
       <c r="F68" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="G68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69">
@@ -2444,13 +2441,13 @@
         <v>39</v>
       </c>
       <c r="E69" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G69" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70">
@@ -2467,13 +2464,13 @@
         <v>40</v>
       </c>
       <c r="E70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G70" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71">
@@ -2493,10 +2490,10 @@
         <v>89</v>
       </c>
       <c r="F71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="72">
@@ -2513,13 +2510,13 @@
         <v>73</v>
       </c>
       <c r="E72" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F72" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G72" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="73">
@@ -2536,13 +2533,13 @@
         <v>40</v>
       </c>
       <c r="E73" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G73" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74">
@@ -2562,10 +2559,10 @@
         <v>9</v>
       </c>
       <c r="F74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75">
@@ -2585,10 +2582,10 @@
         <v>75</v>
       </c>
       <c r="F75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76">
@@ -2608,10 +2605,10 @@
         <v>74</v>
       </c>
       <c r="F76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G76" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="77">
@@ -2631,10 +2628,10 @@
         <v>82</v>
       </c>
       <c r="F77" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G77" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="78">
@@ -2651,13 +2648,13 @@
         <v>39</v>
       </c>
       <c r="E78" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G78" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79">
@@ -2674,13 +2671,13 @@
         <v>40</v>
       </c>
       <c r="E79" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="F79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G79" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="80">
@@ -2697,13 +2694,13 @@
         <v>73</v>
       </c>
       <c r="E80" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G80" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81">
@@ -2720,13 +2717,13 @@
         <v>40</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82">
@@ -2746,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="F82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G82" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>